<commit_message>
submitREQ9482_TST1200  and change with VerifyProperty function
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST964_DeleteDevice.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST964_DeleteDevice.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="270" yWindow="2535" windowWidth="15480" windowHeight="11640"/>
@@ -4003,7 +4003,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4052,6 +4052,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4786,7 +4789,7 @@
   <dimension ref="A1:O110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5035,7 +5038,7 @@
       <c r="A8" s="2" t="s">
         <v>761</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="4">
         <v>7</v>
       </c>

</xml_diff>